<commit_message>
Fixed M_i(L) to N_i(L)
</commit_message>
<xml_diff>
--- a/EX_W9_data.xlsx
+++ b/EX_W9_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteo/Projects/PSSP_notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CC4D81-CBE6-B640-A25E-87379217B8C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F1560F-F73E-C644-B1B7-C0009D52C8B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{A1C123CF-BBA9-FA40-A565-F4C76E1B9435}"/>
   </bookViews>
@@ -57,10 +57,10 @@
     <t>L</t>
   </si>
   <si>
-    <t>MA(L)</t>
+    <t>NA(L)</t>
   </si>
   <si>
-    <t>MB(L)</t>
+    <t>NB(L)</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>